<commit_message>
finished eeuuAnalysis.xlsx - esteban. i have to add the table and the excel to the google drive and automatize it. also started working on subperiod_stats excels
</commit_message>
<xml_diff>
--- a/backtesting/stats.xlsx
+++ b/backtesting/stats.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,16 @@
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
       <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>S&amp;P-500</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -546,6 +556,36 @@
           <t>Min</t>
         </is>
       </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>Mediana</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>Media geo.</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>Media arit.</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>Desvio</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -554,40 +594,58 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="C4" t="n">
         <v>0.09</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.05</v>
-      </c>
       <c r="D4" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="E4" t="n">
-        <v>1.42</v>
+        <v>2.08</v>
       </c>
       <c r="F4" t="n">
-        <v>9.380000000000001</v>
+        <v>11.98</v>
       </c>
       <c r="G4" t="n">
-        <v>-11.98</v>
+        <v>-12.86</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="J4" t="n">
-        <v>0.02</v>
+        <v>0.11</v>
       </c>
       <c r="K4" t="n">
-        <v>1.33</v>
+        <v>2.02</v>
       </c>
       <c r="L4" t="n">
-        <v>11.98</v>
+        <v>12.86</v>
       </c>
       <c r="M4" t="n">
-        <v>-9.380000000000001</v>
+        <v>-11.98</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="R4" t="n">
+        <v>9.380000000000001</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-11.98</v>
       </c>
     </row>
     <row r="5">
@@ -597,39 +655,57 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="C5" t="n">
-        <v>0.05</v>
+        <v>0.18</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06</v>
+        <v>0.19</v>
       </c>
       <c r="E5" t="n">
-        <v>0.83</v>
+        <v>1.68</v>
       </c>
       <c r="F5" t="n">
-        <v>2.62</v>
+        <v>10.47</v>
       </c>
       <c r="G5" t="n">
-        <v>-5.89</v>
+        <v>-8.01</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="I5" t="n">
-        <v>0.05</v>
+        <v>0.18</v>
       </c>
       <c r="J5" t="n">
-        <v>0.06</v>
+        <v>0.19</v>
       </c>
       <c r="K5" t="n">
-        <v>0.83</v>
+        <v>1.68</v>
       </c>
       <c r="L5" t="n">
-        <v>2.62</v>
+        <v>10.47</v>
       </c>
       <c r="M5" t="n">
+        <v>-8.01</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3.41</v>
+      </c>
+      <c r="S5" t="n">
         <v>-5.89</v>
       </c>
     </row>
@@ -640,22 +716,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.04</v>
+        <v>0.37</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="D6" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="E6" t="n">
-        <v>1.5</v>
+        <v>2.02</v>
       </c>
       <c r="F6" t="n">
-        <v>3.41</v>
+        <v>7.56</v>
       </c>
       <c r="G6" t="n">
-        <v>-4.32</v>
+        <v>-3.86</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -674,6 +750,24 @@
       </c>
       <c r="M6" t="n">
         <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2.76</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-2.5</v>
       </c>
     </row>
     <row r="7">
@@ -683,46 +777,65 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="F7" t="n">
+        <v>11.98</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-12.86</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="L7" t="n">
+        <v>12.86</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-11.98</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="P7" t="n">
         <v>0.01</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="Q7" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="R7" t="n">
         <v>9.380000000000001</v>
       </c>
-      <c r="G7" t="n">
+      <c r="S7" t="n">
         <v>-11.98</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-0.01</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2.03</v>
-      </c>
-      <c r="L7" t="n">
-        <v>11.98</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-9.380000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>